<commit_message>
Converted to attended version in order to publish to UiPath Marketplace
</commit_message>
<xml_diff>
--- a/Data/tickersToAddTable.xlsx
+++ b/Data/tickersToAddTable.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23819"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jackc\Desktop\Work\RPA\Own Projects\JackFrameworkBlankV2-WithLibrary\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jackc\Desktop\Work\RPA\Own Projects UiPath\GenerateStockAndCryptoSummary\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1426B6D0-EDFC-4E52-8AFC-68AC30392B10}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A523254-73CB-41AC-99DF-CC8F031723BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10224" yWindow="324" windowWidth="12816" windowHeight="12036" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Data" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,13 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
-  <si>
-    <t>stock</t>
-  </si>
-  <si>
-    <t>crypto</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Type</t>
   </si>
@@ -40,7 +34,10 @@
     <t>Ticker</t>
   </si>
   <si>
-    <t>GME</t>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>Crypto</t>
   </si>
 </sst>
 </file>
@@ -368,32 +365,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.21875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -418,20 +407,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D23B150-86B3-41B3-B117-FFB7177B10D1}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>